<commit_message>
Add unzip test.xlsx and test-original.xlsx files
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,106 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12648" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>a</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>b</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>g</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>h</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>i</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>j</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>k</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>l</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>m</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>o</t>
-    <phoneticPr fontId="1"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="游ゴシック"/>
+      <charset val="128"/>
+      <family val="3"/>
       <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -116,30 +51,89 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="標準" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -405,139 +399,163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
+    <row r="1">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C5" t="n">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D5" t="n">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E5" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s">
+      <c r="F5" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="6">
+      <c r="B6" t="n">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C6" t="n">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D6" t="n">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E6" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
-      <c r="B4" t="s">
+      <c r="F6" t="n">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
+    </row>
+    <row r="7">
       <c r="B7">
         <f>B5+B6</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:F7" si="0">C5+C6</f>
-        <v>9</v>
+        <f>C5+C6</f>
+        <v/>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>D5+D6</f>
+        <v/>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>E5+E6</f>
+        <v/>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>F5+F6</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -547,21 +565,77 @@
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
   </mergeCells>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>